<commit_message>
Add calculation steps and final results partial views, enhance profile edit page with improved UI and validation, update feedback display logic in history views, and modify routes for new functionalities. improve landing page, login, and ergister page. make noticitaion featrue from observer, logout confirm modal. improve SPK calculations should be performed every 3 days if there are changes and can be done manually, with real-time updates. Improve the kategori kerusakan addition feature by adding generate input.
</commit_message>
<xml_diff>
--- a/public/assets/excel/template_data_pengguna.xlsx
+++ b/public/assets/excel/template_data_pengguna.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PBL-Fasilita\public\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7478FBEC-2C75-4E41-B204-5413C1E1359B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD82DABF-B616-4DE3-928C-F93EA57DB035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>id_peran</t>
   </si>
@@ -49,6 +49,15 @@
   </si>
   <si>
     <t>Nadya Siva</t>
+  </si>
+  <si>
+    <t>nomor induk</t>
+  </si>
+  <si>
+    <t>198311052003101000</t>
+  </si>
+  <si>
+    <t>195912312010123890</t>
   </si>
 </sst>
 </file>
@@ -84,8 +93,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,58 +376,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:F7"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="11.1796875" customWidth="1"/>
+    <col min="1" max="1" width="11.1796875" customWidth="1"/>
+    <col min="2" max="2" width="24.26953125" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.26953125" customWidth="1"/>
     <col min="4" max="4" width="11.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>12345</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>12345</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: enhance pengguna management with improved validation and error handling
</commit_message>
<xml_diff>
--- a/public/assets/excel/template_data_pengguna.xlsx
+++ b/public/assets/excel/template_data_pengguna.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PBL-Fasilita\public\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD82DABF-B616-4DE3-928C-F93EA57DB035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616D1E30-0ACF-43AD-A0B3-D513BCBCD3A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,10 +54,10 @@
     <t>nomor induk</t>
   </si>
   <si>
-    <t>198311052003101000</t>
-  </si>
-  <si>
-    <t>195912312010123890</t>
+    <t>198311052003101001</t>
+  </si>
+  <si>
+    <t>195912312010122890</t>
   </si>
 </sst>
 </file>
@@ -379,7 +379,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>